<commit_message>
hardware, orders: update expansions panel bom to match current re-order and remove reference and original BOMs since these are in the archive now
</commit_message>
<xml_diff>
--- a/hardware/orders/pods_panel/bom.xlsx
+++ b/hardware/orders/pods_panel/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\563554\src\RAMN\hardware\orders\pods_panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{086B6E11-5060-4B3A-B5CB-46BFEE907555}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E728C5-CC9D-4CAC-8094-7F2859DB3AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19590" yWindow="-20985" windowWidth="39855" windowHeight="20985" xr2:uid="{DB9C5124-A61E-4353-97B3-5A428009B5E9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB9C5124-A61E-4353-97B3-5A428009B5E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="132">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -261,9 +261,6 @@
   </si>
   <si>
     <t>KNOB SMOOTH 0.157 X 0.079" NYLON</t>
-  </si>
-  <si>
-    <t>1231-M</t>
   </si>
   <si>
     <t>KNOB SERR W/SKIRT 0.236" PLASTIC</t>
@@ -477,6 +474,10 @@
   </si>
   <si>
     <t>10 kOhms 0.05W, 1/20W Through Hole Slide Potentiometer Top Adjustment Type</t>
+  </si>
+  <si>
+    <t>1231-M</t>
+    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1050,8 +1051,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E0B32C-D87D-4064-9431-F8E6EE1E1F78}">
   <dimension ref="A1:J43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1069,7 +1070,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="22" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1082,31 +1083,31 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>104</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>105</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>106</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>107</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="14" t="s">
         <v>108</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>109</v>
       </c>
       <c r="J2" s="16"/>
     </row>
@@ -1136,16 +1137,16 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="J4" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="13" customFormat="1" ht="30.75" thickBot="1">
@@ -1171,13 +1172,13 @@
         <v>10</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
@@ -1200,14 +1201,14 @@
         <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
@@ -1215,7 +1216,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1230,14 +1231,14 @@
         <v>19</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30.75" thickBot="1">
@@ -1260,16 +1261,16 @@
         <v>23</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1">
@@ -1292,16 +1293,16 @@
         <v>26</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1">
@@ -1309,7 +1310,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
@@ -1324,21 +1325,21 @@
         <v>19</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="B11" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1362,16 +1363,16 @@
         <v>2</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30.75" thickBot="1">
@@ -1394,14 +1395,14 @@
         <v>7</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30.75" thickBot="1">
@@ -1424,14 +1425,14 @@
         <v>5</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30.75" thickBot="1">
@@ -1451,19 +1452,19 @@
         <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45.75" thickBot="1">
@@ -1483,17 +1484,17 @@
         <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30.75" thickBot="1">
@@ -1513,17 +1514,17 @@
         <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" ht="45.75" thickBot="1">
@@ -1543,19 +1544,19 @@
         <v>68</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30.75" thickBot="1">
@@ -1575,17 +1576,17 @@
         <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="13" customFormat="1" ht="52.5" customHeight="1" thickBot="1">
@@ -1602,7 +1603,7 @@
         <v>73</v>
       </c>
       <c r="E20" s="21" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F20" s="21" t="s">
         <v>74</v>
@@ -1610,36 +1611,38 @@
       <c r="G20" s="11"/>
       <c r="H20" s="11"/>
       <c r="I20" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A21">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" s="13" customFormat="1" ht="52.5" customHeight="1" thickBot="1">
+      <c r="A21" s="13">
         <v>209</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="B21" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C21" s="2">
-        <v>1</v>
-      </c>
-      <c r="D21" s="1" t="s">
+      <c r="C21" s="12">
+        <v>1</v>
+      </c>
+      <c r="D21" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="E21" s="21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="17" t="s">
-        <v>90</v>
+      <c r="G21" s="11"/>
+      <c r="H21" s="11"/>
+      <c r="I21" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="J21" s="18" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="22" spans="1:10" s="4" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
@@ -1668,16 +1671,16 @@
         <v>2</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H23" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I23" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="J23" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="J23" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1700,14 +1703,14 @@
         <v>7</v>
       </c>
       <c r="G24" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H24" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H24" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I24" s="6"/>
       <c r="J24" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1730,14 +1733,14 @@
         <v>5</v>
       </c>
       <c r="G25" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H25" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H25" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1757,19 +1760,19 @@
         <v>48</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H26" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J26" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="95.25" customHeight="1" thickBot="1">
@@ -1783,23 +1786,23 @@
         <v>2</v>
       </c>
       <c r="D27" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>131</v>
-      </c>
       <c r="G27" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H27" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I27" s="6"/>
       <c r="J27" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1819,17 +1822,17 @@
         <v>56</v>
       </c>
       <c r="F28" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>119</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>120</v>
-      </c>
       <c r="H28" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1837,31 +1840,31 @@
         <v>306</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C29" s="12">
         <v>5</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E29" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F29" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G29" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H29" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I29" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1881,17 +1884,17 @@
         <v>45</v>
       </c>
       <c r="F30" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H30" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I30" s="6"/>
       <c r="J30" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
@@ -1920,16 +1923,16 @@
         <v>2</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H32" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I32" s="6" t="s">
         <v>86</v>
       </c>
-      <c r="I32" s="6" t="s">
+      <c r="J32" s="17" t="s">
         <v>87</v>
-      </c>
-      <c r="J32" s="17" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="30.75" thickBot="1">
@@ -1952,14 +1955,14 @@
         <v>5</v>
       </c>
       <c r="G33" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H33" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H33" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30.75" thickBot="1">
@@ -1982,14 +1985,14 @@
         <v>7</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="15.75" thickBot="1">
@@ -2012,14 +2015,14 @@
         <v>34</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30.75" thickBot="1">
@@ -2036,20 +2039,20 @@
         <v>46</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F36" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G36" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30.75" thickBot="1">
@@ -2066,20 +2069,20 @@
         <v>46</v>
       </c>
       <c r="E37" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F37" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="F37" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="G37" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H37" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I37" s="6"/>
       <c r="J37" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="30.75" thickBot="1">
@@ -2096,20 +2099,20 @@
         <v>46</v>
       </c>
       <c r="E38" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="F38" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="F38" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="G38" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="H38" s="6" t="s">
         <v>83</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>84</v>
       </c>
       <c r="I38" s="6"/>
       <c r="J38" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="30.75" thickBot="1">
@@ -2129,19 +2132,19 @@
         <v>48</v>
       </c>
       <c r="F39" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H39" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="J39" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="15.75" thickBot="1">
@@ -2149,31 +2152,31 @@
         <v>408</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C40" s="12">
         <v>6</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="E40" s="10" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="F40" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G40" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="H40" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I40" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:10" s="13" customFormat="1" ht="33" customHeight="1" thickBot="1">
@@ -2196,16 +2199,16 @@
         <v>43</v>
       </c>
       <c r="G41" s="11" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H41" s="11" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="I41" s="11" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="22.5" customHeight="1" thickBot="1">
@@ -2228,14 +2231,14 @@
         <v>39</v>
       </c>
       <c r="G42" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I42" s="6"/>
       <c r="J42" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="30.75" thickBot="1">
@@ -2255,17 +2258,17 @@
         <v>45</v>
       </c>
       <c r="F43" s="1" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="H43" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I43" s="6"/>
       <c r="J43" s="17" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
hardware, ordering: remove knobs from expansion panel bom
</commit_message>
<xml_diff>
--- a/hardware/orders/pods_panel/bom.xlsx
+++ b/hardware/orders/pods_panel/bom.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\563554\src\RAMN\hardware\orders\pods_panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{63E728C5-CC9D-4CAC-8094-7F2859DB3AEF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D80306-5B49-4AA6-9560-596C5CBD71D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB9C5124-A61E-4353-97B3-5A428009B5E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="127">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -257,20 +257,7 @@
     <t>J7</t>
   </si>
   <si>
-    <t>Davies Molding, LLC</t>
-  </si>
-  <si>
-    <t>KNOB SMOOTH 0.157 X 0.079" NYLON</t>
-  </si>
-  <si>
-    <t>KNOB SERR W/SKIRT 0.236" PLASTIC</t>
-  </si>
-  <si>
     <t>Chassis Pod</t>
-  </si>
-  <si>
-    <t>1300-F</t>
-    <phoneticPr fontId="1"/>
   </si>
   <si>
     <t>J5</t>
@@ -474,10 +461,6 @@
   </si>
   <si>
     <t>10 kOhms 0.05W, 1/20W Through Hole Slide Potentiometer Top Adjustment Type</t>
-  </si>
-  <si>
-    <t>1231-M</t>
-    <phoneticPr fontId="1"/>
   </si>
 </sst>
 </file>
@@ -1049,10 +1032,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E0B32C-D87D-4064-9431-F8E6EE1E1F78}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1070,7 +1053,7 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="B1" s="22" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C1" s="22"/>
       <c r="D1" s="22"/>
@@ -1083,31 +1066,31 @@
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
+        <v>96</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="E2" s="9" t="s">
         <v>100</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="G2" s="9" t="s">
         <v>102</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>103</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="I2" s="14" t="s">
         <v>104</v>
-      </c>
-      <c r="F2" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G2" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>108</v>
       </c>
       <c r="J2" s="16"/>
     </row>
@@ -1137,16 +1120,16 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H4" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="I4" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="5" spans="1:10" s="13" customFormat="1" ht="30.75" thickBot="1">
@@ -1172,13 +1155,13 @@
         <v>10</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I5" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
@@ -1201,14 +1184,14 @@
         <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="6" t="s">
         <v>84</v>
-      </c>
-      <c r="H6" s="6" t="s">
-        <v>88</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
@@ -1216,7 +1199,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1231,14 +1214,14 @@
         <v>19</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30.75" thickBot="1">
@@ -1261,16 +1244,16 @@
         <v>23</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1">
@@ -1293,16 +1276,16 @@
         <v>26</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1">
@@ -1310,7 +1293,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
@@ -1325,21 +1308,21 @@
         <v>19</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="B11" s="3" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1363,16 +1346,16 @@
         <v>2</v>
       </c>
       <c r="G12" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="6" t="s">
-        <v>85</v>
-      </c>
       <c r="I12" s="6" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="J12" s="17" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30.75" thickBot="1">
@@ -1395,14 +1378,14 @@
         <v>7</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H13" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30.75" thickBot="1">
@@ -1425,14 +1408,14 @@
         <v>5</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H14" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30.75" thickBot="1">
@@ -1452,19 +1435,19 @@
         <v>48</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="G15" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H15" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="H15" s="6" t="s">
-        <v>88</v>
-      </c>
       <c r="I15" s="6" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45.75" thickBot="1">
@@ -1484,17 +1467,17 @@
         <v>71</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30.75" thickBot="1">
@@ -1514,17 +1497,17 @@
         <v>65</v>
       </c>
       <c r="F17" s="1" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" ht="45.75" thickBot="1">
@@ -1544,19 +1527,19 @@
         <v>68</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="G18" s="11" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="I18" s="11" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30.75" thickBot="1">
@@ -1576,699 +1559,643 @@
         <v>45</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" s="13" customFormat="1" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A20" s="13">
-        <v>208</v>
-      </c>
-      <c r="B20" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C20" s="12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" s="4" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
+      <c r="B20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="19"/>
+    </row>
+    <row r="21" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+      <c r="B21" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F21" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D20" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E20" s="21" t="s">
+      <c r="G21" s="6" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="21" t="s">
-        <v>74</v>
-      </c>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J20" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" s="13" customFormat="1" ht="52.5" customHeight="1" thickBot="1">
-      <c r="A21" s="13">
-        <v>209</v>
-      </c>
-      <c r="B21" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C21" s="12">
-        <v>1</v>
-      </c>
-      <c r="D21" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="E21" s="21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="G21" s="11"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J21" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" s="4" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
-      <c r="B22" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G22" s="5"/>
-      <c r="H22" s="5"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="19"/>
+      <c r="H21" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J21" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A22">
+        <v>301</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C22" s="2">
+        <v>6</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G22" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I22" s="6"/>
+      <c r="J22" s="17" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="23" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A23">
+        <v>302</v>
+      </c>
       <c r="B23" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>3</v>
+        <v>54</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>9</v>
+        <v>28</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F23" s="1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H23" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I23" s="6" t="s">
-        <v>86</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I23" s="6"/>
       <c r="J23" s="17" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
       <c r="A24">
-        <v>301</v>
+        <v>303</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
       <c r="C24" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>30</v>
+        <v>49</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>7</v>
+        <v>107</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I24" s="6"/>
+        <v>84</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>123</v>
+      </c>
       <c r="J24" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="95.25" customHeight="1" thickBot="1">
       <c r="A25">
-        <v>302</v>
+        <v>304</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>28</v>
+        <v>125</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>4</v>
+        <v>124</v>
       </c>
       <c r="F25" s="1" t="s">
-        <v>5</v>
+        <v>126</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
       <c r="A26">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>61</v>
+        <v>58</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="F26" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G26" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I26" s="6"/>
+      <c r="J26" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
+      <c r="A27">
+        <v>306</v>
+      </c>
+      <c r="B27" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="C27" s="12">
+        <v>5</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G27" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H27" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="H26" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I26" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" ht="95.25" customHeight="1" thickBot="1">
-      <c r="A27">
-        <v>304</v>
-      </c>
-      <c r="B27" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C27" s="2">
-        <v>2</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="F27" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="G27" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="H27" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I27" s="6"/>
-      <c r="J27" s="17" t="s">
-        <v>89</v>
+      <c r="I27" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J27" s="18" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
       <c r="A28">
-        <v>305</v>
+        <v>307</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C28" s="2">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>118</v>
+        <v>108</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>119</v>
+        <v>94</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A29">
-        <v>306</v>
-      </c>
-      <c r="B29" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C29" s="12">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
+      <c r="B29" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="G29" s="5"/>
+      <c r="H29" s="5"/>
+      <c r="I29" s="5"/>
+      <c r="J29" s="19"/>
+    </row>
+    <row r="30" spans="1:10" ht="75.75" thickBot="1">
+      <c r="B30" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H30" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="I30" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="J30" s="17" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" ht="30.75" thickBot="1">
+      <c r="A31">
+        <v>401</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C31" s="2">
+        <v>1</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F31" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D29" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>94</v>
-      </c>
-      <c r="F29" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G29" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H29" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I29" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J29" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
-      <c r="A30">
-        <v>307</v>
-      </c>
-      <c r="B30" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="C30" s="2">
+      <c r="G31" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I31" s="6"/>
+      <c r="J31" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" ht="30.75" thickBot="1">
+      <c r="A32">
+        <v>402</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C32" s="2">
         <v>3</v>
       </c>
-      <c r="D30" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F30" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G30" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H30" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I30" s="6"/>
-      <c r="J30" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
-      <c r="B31" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G31" s="5"/>
-      <c r="H31" s="5"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="19"/>
-    </row>
-    <row r="32" spans="1:10" ht="75.75" thickBot="1">
-      <c r="B32" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>3</v>
-      </c>
       <c r="D32" s="1" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F32" s="1" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G32" s="6" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="H32" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="I32" s="6" t="s">
-        <v>86</v>
-      </c>
+        <v>79</v>
+      </c>
+      <c r="I32" s="6"/>
       <c r="J32" s="17" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" ht="30.75" thickBot="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" ht="15.75" thickBot="1">
       <c r="A33">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="C33" s="2">
         <v>1</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>4</v>
+        <v>32</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30.75" thickBot="1">
       <c r="A34">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C34" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>30</v>
+        <v>46</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>7</v>
+        <v>117</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H34" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" ht="15.75" thickBot="1">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" ht="30.75" thickBot="1">
       <c r="A35">
-        <v>403</v>
+        <v>405</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>35</v>
+        <v>51</v>
       </c>
       <c r="C35" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>33</v>
+        <v>46</v>
       </c>
       <c r="E35" s="1" t="s">
-        <v>32</v>
+        <v>119</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>34</v>
+        <v>120</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>109</v>
+        <v>78</v>
       </c>
       <c r="H35" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30.75" thickBot="1">
       <c r="A36">
-        <v>404</v>
+        <v>406</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>36</v>
+        <v>52</v>
       </c>
       <c r="C36" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
         <v>46</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>121</v>
-      </c>
       <c r="G36" s="6" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="17" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30.75" thickBot="1">
       <c r="A37">
-        <v>405</v>
+        <v>407</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C37" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E37" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="F37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="I37" s="6" t="s">
+        <v>123</v>
+      </c>
+      <c r="J37" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" ht="15.75" thickBot="1">
+      <c r="A38">
+        <v>408</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C38" s="12">
+        <v>6</v>
+      </c>
+      <c r="D38" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="G38" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="H38" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I38" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J38" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" s="13" customFormat="1" ht="33" customHeight="1" thickBot="1">
+      <c r="A39">
+        <v>409</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C39" s="12">
+        <v>1</v>
+      </c>
+      <c r="D39" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E39" s="21" t="s">
+        <v>41</v>
+      </c>
+      <c r="F39" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="G39" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="H39" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="I39" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="J39" s="18" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" ht="22.5" customHeight="1" thickBot="1">
+      <c r="A40">
+        <v>410</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C40" s="2">
+        <v>1</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="F40" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G40" s="6" t="s">
+        <v>106</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I40" s="6"/>
+      <c r="J40" s="17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" ht="30.75" thickBot="1">
+      <c r="A41">
+        <v>411</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="E37" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="F37" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="G37" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I37" s="6"/>
-      <c r="J37" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A38">
-        <v>406</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>52</v>
-      </c>
-      <c r="C38" s="2">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="F38" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="G38" s="6" t="s">
-        <v>82</v>
-      </c>
-      <c r="H38" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I38" s="6"/>
-      <c r="J38" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A39">
-        <v>407</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="2">
-        <v>1</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="F39" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="G39" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="H39" s="6" t="s">
-        <v>88</v>
-      </c>
-      <c r="I39" s="6" t="s">
-        <v>127</v>
-      </c>
-      <c r="J39" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A40">
-        <v>408</v>
-      </c>
-      <c r="B40" s="10" t="s">
-        <v>120</v>
-      </c>
-      <c r="C40" s="12">
-        <v>6</v>
-      </c>
-      <c r="D40" s="10" t="s">
-        <v>95</v>
-      </c>
-      <c r="E40" s="10" t="s">
+      <c r="E41" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G41" s="6" t="s">
         <v>94</v>
       </c>
-      <c r="F40" s="10" t="s">
-        <v>93</v>
-      </c>
-      <c r="G40" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="H40" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I40" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J40" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" s="13" customFormat="1" ht="33" customHeight="1" thickBot="1">
-      <c r="A41">
-        <v>409</v>
-      </c>
-      <c r="B41" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C41" s="12">
-        <v>1</v>
-      </c>
-      <c r="D41" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E41" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F41" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G41" s="11" t="s">
-        <v>96</v>
-      </c>
-      <c r="H41" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="I41" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="J41" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" ht="22.5" customHeight="1" thickBot="1">
-      <c r="A42">
-        <v>410</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="2">
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F42" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="G42" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="H42" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I42" s="6"/>
-      <c r="J42" s="17" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" ht="30.75" thickBot="1">
-      <c r="A43">
-        <v>411</v>
-      </c>
-      <c r="B43" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="2">
-        <v>1</v>
-      </c>
-      <c r="D43" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="E43" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="F43" s="1" t="s">
-        <v>112</v>
-      </c>
-      <c r="G43" s="6" t="s">
-        <v>98</v>
-      </c>
-      <c r="H43" s="6" t="s">
-        <v>83</v>
-      </c>
-      <c r="I43" s="6"/>
-      <c r="J43" s="17" t="s">
-        <v>89</v>
+      <c r="H41" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="I41" s="6"/>
+      <c r="J41" s="17" t="s">
+        <v>85</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
orders, pcbway: update pods panel bom to reflect new parts availability from PCBWay (all parts are now available)
</commit_message>
<xml_diff>
--- a/hardware/orders/pods_panel/bom.xlsx
+++ b/hardware/orders/pods_panel/bom.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\563554\src\RAMN\hardware\orders\pods_panel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91D80306-5B49-4AA6-9560-596C5CBD71D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD34312F-E8C8-4E67-9A65-B3D09AAC5A4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{DB9C5124-A61E-4353-97B3-5A428009B5E9}"/>
+    <workbookView xWindow="-2610" yWindow="-21600" windowWidth="39855" windowHeight="20985" xr2:uid="{DB9C5124-A61E-4353-97B3-5A428009B5E9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="127">
   <si>
     <t>Reference Designator</t>
   </si>
@@ -159,9 +159,6 @@
   </si>
   <si>
     <t>U1</t>
-  </si>
-  <si>
-    <t>SK14EG13</t>
   </si>
   <si>
     <t>NKK Switches</t>
@@ -461,6 +458,9 @@
   </si>
   <si>
     <t>10 kOhms 0.05W, 1/20W Through Hole Slide Potentiometer Top Adjustment Type</t>
+  </si>
+  <si>
+    <t>SK14DG13 (OR SK14EG13)</t>
   </si>
 </sst>
 </file>
@@ -524,7 +524,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -547,12 +547,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -661,7 +655,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -707,12 +701,25 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1034,8 +1041,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{94E0B32C-D87D-4064-9431-F8E6EE1E1F78}">
   <dimension ref="A1:J41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1052,45 +1059,45 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
-      <c r="B1" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
+      <c r="B1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
     </row>
     <row r="2" spans="1:10">
       <c r="A2" s="8" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2" s="9" t="s">
         <v>96</v>
       </c>
-      <c r="B2" s="9" t="s">
+      <c r="C2" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="D2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="E2" s="9" t="s">
         <v>99</v>
       </c>
-      <c r="E2" s="9" t="s">
+      <c r="F2" s="8" t="s">
         <v>100</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="G2" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="H2" s="8" t="s">
         <v>102</v>
       </c>
-      <c r="H2" s="8" t="s">
+      <c r="I2" s="14" t="s">
         <v>103</v>
-      </c>
-      <c r="I2" s="14" t="s">
-        <v>104</v>
       </c>
       <c r="J2" s="16"/>
     </row>
@@ -1120,48 +1127,46 @@
         <v>2</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H4" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I4" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I4" s="6" t="s">
+      <c r="J4" s="17" t="s">
         <v>82</v>
       </c>
-      <c r="J4" s="17" t="s">
+    </row>
+    <row r="5" spans="1:10" s="13" customFormat="1" ht="30.75" thickBot="1">
+      <c r="A5" s="27">
+        <v>101</v>
+      </c>
+      <c r="B5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="23">
+        <v>1</v>
+      </c>
+      <c r="D5" s="26" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="26">
+        <v>4313</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="24" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" s="13" customFormat="1" ht="30.75" thickBot="1">
-      <c r="A5" s="13">
-        <v>101</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="12">
-        <v>1</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="21">
-        <v>4313</v>
-      </c>
-      <c r="F5" s="21" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I5" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J5" s="18" t="s">
-        <v>85</v>
+      <c r="I5" s="24"/>
+      <c r="J5" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="15.75" thickBot="1">
@@ -1184,14 +1189,14 @@
         <v>16</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I6" s="6"/>
       <c r="J6" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" thickBot="1">
@@ -1199,7 +1204,7 @@
         <v>103</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C7" s="2">
         <v>1</v>
@@ -1214,14 +1219,14 @@
         <v>19</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H7" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I7" s="6"/>
       <c r="J7" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="30.75" thickBot="1">
@@ -1244,16 +1249,16 @@
         <v>23</v>
       </c>
       <c r="G8" s="11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I8" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="9" spans="1:10" ht="15.75" thickBot="1">
@@ -1276,16 +1281,16 @@
         <v>26</v>
       </c>
       <c r="G9" s="11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I9" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J9" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:10" ht="15.75" thickBot="1">
@@ -1293,7 +1298,7 @@
         <v>106</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C10" s="12">
         <v>1</v>
@@ -1308,21 +1313,21 @@
         <v>19</v>
       </c>
       <c r="G10" s="11" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I10" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
       <c r="B11" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="5"/>
@@ -1346,16 +1351,16 @@
         <v>2</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H12" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I12" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I12" s="6" t="s">
+      <c r="J12" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="J12" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="13" spans="1:10" ht="30.75" thickBot="1">
@@ -1363,7 +1368,7 @@
         <v>201</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C13" s="2">
         <v>5</v>
@@ -1378,14 +1383,14 @@
         <v>7</v>
       </c>
       <c r="G13" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H13" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H13" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I13" s="6"/>
       <c r="J13" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="14" spans="1:10" ht="30.75" thickBot="1">
@@ -1393,7 +1398,7 @@
         <v>202</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="2">
         <v>1</v>
@@ -1408,14 +1413,14 @@
         <v>5</v>
       </c>
       <c r="G14" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H14" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I14" s="6"/>
       <c r="J14" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="30.75" thickBot="1">
@@ -1423,31 +1428,31 @@
         <v>203</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" s="2">
         <v>1</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J15" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="45.75" thickBot="1">
@@ -1455,29 +1460,29 @@
         <v>204</v>
       </c>
       <c r="B16" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C16" s="2">
+        <v>1</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="C16" s="2">
-        <v>1</v>
-      </c>
-      <c r="D16" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="F16" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I16" s="6"/>
       <c r="J16" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="30.75" thickBot="1">
@@ -1485,61 +1490,59 @@
         <v>205</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C17" s="2">
+        <v>1</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="C17" s="2">
-        <v>1</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>65</v>
-      </c>
       <c r="F17" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="G17" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I17" s="6"/>
       <c r="J17" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:10" s="13" customFormat="1" ht="45.75" thickBot="1">
       <c r="A18">
         <v>206</v>
       </c>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="22" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="23">
+        <v>1</v>
+      </c>
+      <c r="D18" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C18" s="12">
-        <v>1</v>
-      </c>
-      <c r="D18" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="F18" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="G18" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H18" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J18" s="18" t="s">
-        <v>85</v>
+      <c r="F18" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="G18" s="24" t="s">
+        <v>108</v>
+      </c>
+      <c r="H18" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="24"/>
+      <c r="J18" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="30.75" thickBot="1">
@@ -1547,34 +1550,34 @@
         <v>207</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C19" s="2">
         <v>3</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F19" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H19" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I19" s="6"/>
       <c r="J19" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="20" spans="1:10" s="4" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
       <c r="B20" s="3" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="5"/>
       <c r="H20" s="5"/>
@@ -1598,16 +1601,16 @@
         <v>2</v>
       </c>
       <c r="G21" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H21" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I21" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I21" s="6" t="s">
+      <c r="J21" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="J21" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="22" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1615,7 +1618,7 @@
         <v>301</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C22" s="2">
         <v>6</v>
@@ -1630,14 +1633,14 @@
         <v>7</v>
       </c>
       <c r="G22" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H22" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H22" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I22" s="6"/>
       <c r="J22" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1645,7 +1648,7 @@
         <v>302</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C23" s="2">
         <v>2</v>
@@ -1660,14 +1663,14 @@
         <v>5</v>
       </c>
       <c r="G23" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H23" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I23" s="6"/>
       <c r="J23" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="24" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1675,31 +1678,31 @@
         <v>303</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C24" s="2">
         <v>1</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F24" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J24" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="25" spans="1:10" ht="95.25" customHeight="1" thickBot="1">
@@ -1707,29 +1710,29 @@
         <v>304</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C25" s="2">
         <v>2</v>
       </c>
       <c r="D25" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F25" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="E25" s="1" t="s">
-        <v>124</v>
-      </c>
-      <c r="F25" s="1" t="s">
-        <v>126</v>
-      </c>
       <c r="G25" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="H25" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I25" s="6"/>
       <c r="J25" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="26" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1737,29 +1740,29 @@
         <v>305</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="2">
         <v>1</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="F26" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G26" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="G26" s="6" t="s">
-        <v>115</v>
-      </c>
       <c r="H26" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I26" s="6"/>
       <c r="J26" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1767,31 +1770,31 @@
         <v>306</v>
       </c>
       <c r="B27" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C27" s="12">
         <v>5</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E27" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F27" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G27" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H27" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I27" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="29.25" customHeight="1" thickBot="1">
@@ -1799,29 +1802,29 @@
         <v>307</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C28" s="2">
         <v>3</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H28" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I28" s="6"/>
       <c r="J28" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:10" s="4" customFormat="1" ht="15.75" thickBot="1">
@@ -1850,16 +1853,16 @@
         <v>2</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H30" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="I30" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="6" t="s">
+      <c r="J30" s="17" t="s">
         <v>82</v>
-      </c>
-      <c r="J30" s="17" t="s">
-        <v>83</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="30.75" thickBot="1">
@@ -1882,14 +1885,14 @@
         <v>5</v>
       </c>
       <c r="G31" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H31" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H31" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I31" s="6"/>
       <c r="J31" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="30.75" thickBot="1">
@@ -1912,14 +1915,14 @@
         <v>7</v>
       </c>
       <c r="G32" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H32" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H32" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I32" s="6"/>
       <c r="J32" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="15.75" thickBot="1">
@@ -1942,14 +1945,14 @@
         <v>34</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="H33" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I33" s="6"/>
       <c r="J33" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="30.75" thickBot="1">
@@ -1963,23 +1966,23 @@
         <v>5</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F34" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="G34" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H34" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H34" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I34" s="6"/>
       <c r="J34" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="30.75" thickBot="1">
@@ -1987,29 +1990,29 @@
         <v>405</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C35" s="2">
         <v>2</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E35" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="F35" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="F35" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="G35" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H35" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H35" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I35" s="6"/>
       <c r="J35" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="30.75" thickBot="1">
@@ -2017,29 +2020,29 @@
         <v>406</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C36" s="2">
         <v>1</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E36" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="F36" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="F36" s="1" t="s">
-        <v>122</v>
-      </c>
       <c r="G36" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="H36" s="6" t="s">
         <v>78</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>79</v>
       </c>
       <c r="I36" s="6"/>
       <c r="J36" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="30.75" thickBot="1">
@@ -2047,31 +2050,31 @@
         <v>407</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C37" s="2">
         <v>1</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F37" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="G37" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="J37" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="15.75" thickBot="1">
@@ -2079,63 +2082,61 @@
         <v>408</v>
       </c>
       <c r="B38" s="10" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C38" s="12">
         <v>6</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E38" s="10" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="F38" s="10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="H38" s="11" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="I38" s="11" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:10" s="13" customFormat="1" ht="33" customHeight="1" thickBot="1">
       <c r="A39">
         <v>409</v>
       </c>
-      <c r="B39" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="C39" s="12">
-        <v>1</v>
-      </c>
-      <c r="D39" s="21" t="s">
+      <c r="B39" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="C39" s="23">
+        <v>1</v>
+      </c>
+      <c r="D39" s="26" t="s">
+        <v>41</v>
+      </c>
+      <c r="E39" s="26" t="s">
+        <v>126</v>
+      </c>
+      <c r="F39" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="E39" s="21" t="s">
-        <v>41</v>
-      </c>
-      <c r="F39" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="G39" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="H39" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="I39" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="J39" s="18" t="s">
-        <v>85</v>
+      <c r="G39" s="24" t="s">
+        <v>91</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="I39" s="24"/>
+      <c r="J39" s="25" t="s">
+        <v>84</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="22.5" customHeight="1" thickBot="1">
@@ -2158,14 +2159,14 @@
         <v>39</v>
       </c>
       <c r="G40" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="H40" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I40" s="6"/>
       <c r="J40" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="30.75" thickBot="1">
@@ -2173,29 +2174,29 @@
         <v>411</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C41" s="2">
         <v>1</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F41" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="G41" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H41" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I41" s="6"/>
       <c r="J41" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>